<commit_message>
mejorando carga de excel y validaciones de dias habiles
</commit_message>
<xml_diff>
--- a/agendas.xlsx
+++ b/agendas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alonso\Desktop\ARIZONA GIT\DJANGO EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alonso\Desktop\ARIZONA GIT\DJANGO EXCEL\DJANGO-EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39331C6-D43D-45B9-8961-37742E0D332B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58034EA4-1163-4CE7-AADA-5FDECC78A797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24B23E80-0095-43EB-B892-898D1CC48C3B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>tipo_cancha</t>
   </si>
@@ -130,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -144,16 +144,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -258,16 +261,39 @@
           <bgColor rgb="FF444654"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFD9D9E3"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="medium">
           <color rgb="FFD9D9E3"/>
         </left>
         <right style="medium">
           <color rgb="FFD9D9E3"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="medium">
+          <color rgb="FFD9D9E3"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFD9D9E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FFD9D9E3"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -293,39 +319,16 @@
           <bgColor rgb="FF444654"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFD9D9E3"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FFD9D9E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color rgb="FFD9D9E3"/>
         </left>
         <right style="medium">
           <color rgb="FFD9D9E3"/>
         </right>
-        <top style="medium">
-          <color rgb="FFD9D9E3"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FFD9D9E3"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -342,10 +345,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9260B6F-05E9-4EB7-8DC6-9B46BF50771A}" name="Tabla1" displayName="Tabla1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="4" tableBorderDxfId="5">
-  <autoFilter ref="A1:C4" xr:uid="{C9260B6F-05E9-4EB7-8DC6-9B46BF50771A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9260B6F-05E9-4EB7-8DC6-9B46BF50771A}" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C6" xr:uid="{C9260B6F-05E9-4EB7-8DC6-9B46BF50771A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{68F0E37C-214C-4AF4-9B20-91C6550E8876}" name="tipo_cancha" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{68F0E37C-214C-4AF4-9B20-91C6550E8876}" name="tipo_cancha" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{790EA924-5A02-4CB9-92E3-353CD0519F6C}" name="dia" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{341847EE-16CD-401C-B704-ADA8172B4BFF}" name="horario" dataDxfId="0"/>
   </tableColumns>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEACA622-A05B-4E11-8641-7E57873D564B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>45012</v>
+        <v>45010</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -705,6 +708,28 @@
       </c>
       <c r="C4" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45009</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45011</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>